<commit_message>
Published state of ETDataset on 25 July 2014.
</commit_message>
<xml_diff>
--- a/source_analyses/eu/2012/2_power_and_heat_plant/wind_source_analysis.xlsx
+++ b/source_analyses/eu/2012/2_power_and_heat_plant/wind_source_analysis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="14840" tabRatio="500" activeTab="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="38">
   <si>
     <t>France</t>
   </si>
@@ -124,25 +124,16 @@
     <t>share coastal</t>
   </si>
   <si>
-    <t>For all datasets except nl, we cannot distinguish between onshore and coastal. We decided to set the share of coastal to 0.</t>
-  </si>
-  <si>
-    <t>Wind turbine coastal</t>
-  </si>
-  <si>
-    <t>Wind turbine offshore</t>
-  </si>
-  <si>
-    <t>Wind turbine inland</t>
-  </si>
-  <si>
-    <t>For the nl dataset, we use the 2011 shares to calculate which share of onshore + coastal goes to onshore and which share goes to coastal.</t>
-  </si>
-  <si>
     <t>average inland + coastal installed capacity</t>
   </si>
   <si>
     <t>share inland</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>see: ../nl/2012/2_power_and_heat_plant/2_chp_pp_source_analysis.xlsx</t>
   </si>
 </sst>
 </file>
@@ -151,7 +142,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -221,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,14 +231,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -380,34 +365,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -431,7 +388,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -487,17 +444,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1674,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H25"/>
+  <dimension ref="A2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1690,7 +1639,7 @@
     <col min="7" max="7" width="37.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
+    <row r="2" spans="1:8">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1707,11 +1656,11 @@
         <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="1:8">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1724,7 +1673,7 @@
         <v>30989</v>
       </c>
       <c r="E3" s="1">
-        <f>AVERAGE(C3,D3)</f>
+        <f t="shared" ref="E3:E9" si="0">AVERAGE(C3,D3)</f>
         <v>29840.5</v>
       </c>
       <c r="F3">
@@ -1732,11 +1681,11 @@
         <v>400.15</v>
       </c>
       <c r="G3" s="1">
-        <f>E3-F3</f>
+        <f t="shared" ref="G3:G9" si="1">E3-F3</f>
         <v>29440.35</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="1:8">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -1749,7 +1698,7 @@
         <v>22784</v>
       </c>
       <c r="E4" s="1">
-        <f>AVERAGE(C4,D4)</f>
+        <f t="shared" si="0"/>
         <v>22229</v>
       </c>
       <c r="F4">
@@ -1757,11 +1706,11 @@
         <v>2.5</v>
       </c>
       <c r="G4" s="1">
-        <f>E4-F4</f>
+        <f t="shared" si="1"/>
         <v>22226.5</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="1:8">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -1774,7 +1723,7 @@
         <v>106454</v>
       </c>
       <c r="E5" s="1">
-        <f>AVERAGE(C5,D5)</f>
+        <f t="shared" si="0"/>
         <v>100403</v>
       </c>
       <c r="F5">
@@ -1782,11 +1731,11 @@
         <v>5778.5</v>
       </c>
       <c r="G5" s="1">
-        <f>E5-F5</f>
+        <f t="shared" si="1"/>
         <v>94624.5</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="1:8">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -1799,7 +1748,7 @@
         <v>7623</v>
       </c>
       <c r="E6" s="1">
-        <f>AVERAGE(C6,D6)</f>
+        <f t="shared" si="0"/>
         <v>7216</v>
       </c>
       <c r="F6">
@@ -1807,11 +1756,11 @@
         <v>0</v>
       </c>
       <c r="G6" s="1">
-        <f>E6-F6</f>
+        <f t="shared" si="1"/>
         <v>7216</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="1:8">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -1824,7 +1773,7 @@
         <v>2391</v>
       </c>
       <c r="E7" s="1">
-        <f>AVERAGE(C7,D7)</f>
+        <f t="shared" si="0"/>
         <v>2331.5</v>
       </c>
       <c r="F7">
@@ -1832,11 +1781,11 @@
         <v>246.9</v>
       </c>
       <c r="G7" s="1">
-        <f>E7-F7</f>
+        <f t="shared" si="1"/>
         <v>2084.6</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="1:8">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -1849,7 +1798,7 @@
         <v>2496</v>
       </c>
       <c r="E8" s="1">
-        <f>AVERAGE(C8,D8)</f>
+        <f t="shared" si="0"/>
         <v>2056</v>
       </c>
       <c r="F8">
@@ -1857,11 +1806,11 @@
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <f>E8-F8</f>
+        <f t="shared" si="1"/>
         <v>2056</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="1:8">
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -1874,7 +1823,7 @@
         <v>8649</v>
       </c>
       <c r="E9" s="1">
-        <f>AVERAGE(C9,D9)</f>
+        <f t="shared" si="0"/>
         <v>7617</v>
       </c>
       <c r="F9">
@@ -1882,11 +1831,11 @@
         <v>3314.45</v>
       </c>
       <c r="G9" s="1">
-        <f>E9-F9</f>
+        <f t="shared" si="1"/>
         <v>4302.55</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="1:8">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1897,13 +1846,13 @@
         <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="1:8">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -1923,7 +1872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="1:8">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -1931,19 +1880,19 @@
         <v>0</v>
       </c>
       <c r="D13" s="30">
-        <f t="shared" ref="D13:D18" si="0">F4/E4</f>
+        <f t="shared" ref="D13:D16" si="2">F4/E4</f>
         <v>1.1246569796212156E-4</v>
       </c>
       <c r="E13" s="30">
-        <f t="shared" ref="E13:E18" si="1">G4/E4</f>
+        <f t="shared" ref="E13:E15" si="3">G4/E4</f>
         <v>0.99988753430203792</v>
       </c>
       <c r="F13" s="31">
-        <f t="shared" ref="F13:F18" si="2">SUM(C13:E13)</f>
+        <f t="shared" ref="F13:F18" si="4">SUM(C13:E13)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="1:8">
       <c r="B14" t="s">
         <v>14</v>
       </c>
@@ -1951,19 +1900,19 @@
         <v>0</v>
       </c>
       <c r="D14" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.7553061163511048E-2</v>
       </c>
       <c r="E14" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.942446938836489</v>
       </c>
       <c r="F14" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="1:8">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -1971,38 +1920,31 @@
         <v>0</v>
       </c>
       <c r="D15" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E15" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F15" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="30">
-        <f>D23/(D23+D25)*G7/E7</f>
-        <v>0.14297104561016319</v>
-      </c>
-      <c r="D16" s="30">
-        <f t="shared" si="0"/>
-        <v>0.1058974908856959</v>
-      </c>
-      <c r="E16" s="30">
-        <f>D25/(D23+D25)*G7/E7</f>
-        <v>0.75113146350414084</v>
-      </c>
-      <c r="F16" s="31">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
+      <c r="C16" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" t="s">
@@ -2012,15 +1954,15 @@
         <v>0</v>
       </c>
       <c r="D17" s="30">
-        <f t="shared" si="0"/>
+        <f>F8/E8</f>
         <v>0</v>
       </c>
       <c r="E17" s="30">
-        <f t="shared" si="1"/>
+        <f>G8/E8</f>
         <v>1</v>
       </c>
       <c r="F17" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2032,68 +1974,21 @@
         <v>0</v>
       </c>
       <c r="D18" s="30">
-        <f t="shared" si="0"/>
+        <f>F9/E9</f>
         <v>0.43513850597348036</v>
       </c>
       <c r="E18" s="30">
-        <f t="shared" si="1"/>
+        <f>G9/E9</f>
         <v>0.56486149402651964</v>
       </c>
       <c r="F18" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="16" thickBot="1"/>
-    <row r="23" spans="2:6" ht="16" thickBot="1">
-      <c r="B23" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="33">
-        <v>0.13400000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="16" thickBot="1">
-      <c r="B24" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="33">
-        <v>0.16200000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="16" thickBot="1">
-      <c r="B25" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="34">
-        <v>0.70399999999999996</v>
-      </c>
-    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23:D25">
-      <formula1>0</formula1>
-      <formula2>1</formula2>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <ignoredErrors>
-    <ignoredError sqref="E16" formula="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>